<commit_message>
Customer-Controller Test (회원계정 관련) (변경- test 후 롤백 추가) _ API Ver 1.1
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cafe24\eclipse-workspace\ShoppingMall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B03A371-79E7-4CA2-BCD9-F2ABC3C86E14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C4BBA7-0A3F-484A-9114-DFA931F52E38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="7200" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="128">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -299,26 +299,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원가입 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원정보수정 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원탈퇴 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디 중복확인 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>장바구니추가 API -</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -470,6 +450,197 @@
   </si>
   <si>
     <t>주문 교환신청 취소 API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/order/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/customer/terms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/order/change</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/admin/goods/image</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/admin/goods/option</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/admin/orderlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/admin/ordercancellist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/admin/member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/admin/displaycategory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/admin/maindisplay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>1H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">아이디 중복확인 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">회원가입 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>로그인 API -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">회원정보수정 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/customer/account/pw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">회원비밀번호 수정 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">회원탈퇴 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -478,9 +649,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +671,15 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -534,7 +714,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -551,16 +731,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -876,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
-  <dimension ref="A2:L51"/>
+  <dimension ref="A2:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -888,8 +1074,9 @@
     <col min="2" max="2" width="21.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="6" max="6" width="10.625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
   </cols>
@@ -910,13 +1097,13 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -940,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -948,11 +1135,17 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>43662</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>56</v>
+      </c>
+      <c r="H3" s="7">
+        <v>43662</v>
+      </c>
+      <c r="I3" t="s">
+        <v>121</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
@@ -964,7 +1157,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -972,511 +1165,924 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <v>43662</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="H4" s="7">
+        <v>43662</v>
+      </c>
+      <c r="I4" t="s">
+        <v>123</v>
+      </c>
       <c r="K4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+      <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="7">
+        <v>125</v>
+      </c>
+      <c r="F5" s="8">
         <v>43662</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="7">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8">
         <v>43662</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="7">
+        <v>8</v>
+      </c>
+      <c r="F7" s="8">
         <v>43662</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="H7" s="7">
+        <v>43662</v>
+      </c>
+      <c r="I7" t="s">
+        <v>123</v>
+      </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="8">
+        <v>43662</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="7">
+        <v>43662</v>
+      </c>
+      <c r="I8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="8">
+        <v>43663</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="8">
+        <v>43663</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+      <c r="C11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="8">
+        <v>43663</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="K12" s="4" t="s">
+      <c r="F13" s="7">
+        <v>43663</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="6"/>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="K13" t="s">
+      <c r="F14" s="7">
+        <v>43664</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="10"/>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="K14" t="s">
+      <c r="F15" s="7">
+        <v>43664</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="K15" t="s">
+      <c r="F16" s="7">
+        <v>43664</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="33" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+    <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="7">
+        <v>43665</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="10"/>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="K17" t="s">
+      <c r="F18" s="7">
+        <v>43665</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="19" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>47</v>
+      <c r="E19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="7">
+        <v>43665</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="7">
+        <v>43666</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="7">
+        <v>43666</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="7">
+        <v>43666</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="7">
+        <v>43666</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="7">
+        <v>43666</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" t="s">
-        <v>61</v>
+      <c r="F25" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="F26" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
         <v>60</v>
+      </c>
+      <c r="F27" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
       <c r="C32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="D32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="3"/>
       <c r="C33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="3"/>
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="7">
+        <v>43668</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>38</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>46</v>
-      </c>
-      <c r="E34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="5"/>
-      <c r="C35" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" t="s">
-        <v>48</v>
       </c>
       <c r="E35" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
+      <c r="F35" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="9"/>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E36" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="5"/>
+      <c r="F36" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="9"/>
       <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="9"/>
+      <c r="C38" t="s">
         <v>41</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>46</v>
-      </c>
-      <c r="E37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="5"/>
-      <c r="C38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" t="s">
-        <v>48</v>
       </c>
       <c r="E38" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="5"/>
+      <c r="F38" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="9"/>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E39" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="5"/>
+      <c r="F39" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="9"/>
       <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="9"/>
+      <c r="C41" t="s">
         <v>44</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>47</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
+      <c r="F41" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="4"/>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="4"/>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="7">
+        <v>43669</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" t="s">
+        <v>112</v>
+      </c>
+      <c r="F44" s="7">
+        <v>43670</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="B43" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D45" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="7">
+        <v>43670</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" s="7">
+        <v>43670</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="C47" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" t="s">
+        <v>113</v>
+      </c>
+      <c r="F47" s="7">
+        <v>43670</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="C48" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
+      <c r="D48" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" s="7">
+        <v>43670</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="C49" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
+      <c r="D49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" s="7">
+        <v>43671</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C50" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" t="s">
+        <v>114</v>
+      </c>
+      <c r="F50" s="7">
+        <v>43671</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C51" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="C46" s="4" t="s">
+      <c r="D51" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" s="7">
+        <v>43671</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C52" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="C47" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="C48" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="4" t="s">
-        <v>102</v>
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" s="7">
+        <v>43671</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B35:B41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Admin-Controller Test (관리자 상품관리 완료) _ API Ver 1.5
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cafe24\eclipse-workspace\ShoppingMall\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9AF1FB-9DEC-4083-A2E5-1DEE0DC8815C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{20A9AE53-4538-43BB-ADEC-93F37BE5EEED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="29070" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="144">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,22 +229,6 @@
   </si>
   <si>
     <t>상품상세조회API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 상품등록 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 상품조회 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 상품수정 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 상품삭제 API -</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -802,6 +782,26 @@
   </si>
   <si>
     <t xml:space="preserve"> [링크](#13-관리자-카테고리-목록-조회-API) </t>
+  </si>
+  <si>
+    <t>관리자 상품등록 API (완)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 상품수정 API (완)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 상품삭제 API (완)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 상품상세조회 API -</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 상품리스트조회 API -</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -880,7 +880,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -907,6 +907,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1228,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
-  <dimension ref="A2:K55"/>
+  <dimension ref="A2:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1279,7 +1282,7 @@
         <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
@@ -1290,7 +1293,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -1308,15 +1311,15 @@
         <v>43662</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1334,41 +1337,41 @@
         <v>43662</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F5" s="5">
         <v>43662</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H5" s="4">
         <v>43662</v>
       </c>
       <c r="I5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1386,15 +1389,15 @@
         <v>43662</v>
       </c>
       <c r="I6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1412,15 +1415,15 @@
         <v>43662</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1432,77 +1435,77 @@
         <v>43662</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H8" s="4">
         <v>43662</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="5"/>
       <c r="G12" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
@@ -1518,12 +1521,12 @@
         <v>43669</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" t="s">
         <v>44</v>
       </c>
@@ -1537,11 +1540,11 @@
         <v>43669</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" t="s">
         <v>45</v>
       </c>
@@ -1555,11 +1558,11 @@
         <v>43670</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
+      <c r="B16" s="11"/>
       <c r="C16" t="s">
         <v>46</v>
       </c>
@@ -1573,11 +1576,11 @@
         <v>43670</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
@@ -1593,12 +1596,12 @@
         <v>43665</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" t="s">
         <v>48</v>
       </c>
@@ -1612,115 +1615,115 @@
         <v>43665</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F19" s="4">
         <v>43668</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" s="4">
         <v>43668</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F21" s="4">
         <v>43668</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4">
         <v>43669</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F23" s="4">
         <v>43669</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F24" s="4">
         <v>43669</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1740,16 +1743,17 @@
         <v>43665</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="9"/>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
         <v>40</v>
@@ -1758,34 +1762,36 @@
         <v>43665</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6"/>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>142</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F27" s="8">
         <v>43665</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
         <v>39</v>
@@ -1794,158 +1800,154 @@
         <v>43665</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
-        <v>123</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="8">
+        <v>43665</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
         <v>4</v>
       </c>
-      <c r="E29" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="4">
-        <v>43668</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="6"/>
-      <c r="C30" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" t="s">
-        <v>81</v>
-      </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F30" s="4">
         <v>43668</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6"/>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F31" s="4">
         <v>43668</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" t="s">
         <v>83</v>
-      </c>
-      <c r="E32" t="s">
-        <v>88</v>
       </c>
       <c r="F32" s="4">
         <v>43668</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F33" s="4">
         <v>43668</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F34" s="4">
         <v>43668</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="6"/>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="4">
+        <v>43668</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C35" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" t="s">
         <v>25</v>
-      </c>
-      <c r="E35" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35" s="4">
-        <v>43663</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H35" s="4">
-        <v>43663</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B36" s="9"/>
-      <c r="C36" t="s">
-        <v>119</v>
-      </c>
-      <c r="D36" t="s">
-        <v>27</v>
       </c>
       <c r="E36" t="s">
         <v>36</v>
@@ -1954,25 +1956,28 @@
         <v>43663</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="H36" s="4">
         <v>43663</v>
       </c>
-      <c r="I36" t="s">
-        <v>118</v>
-      </c>
-      <c r="J36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="9"/>
+      <c r="I36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E37" t="s">
         <v>36</v>
@@ -1981,7 +1986,7 @@
         <v>43663</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H37" s="4">
         <v>43663</v>
@@ -1990,49 +1995,46 @@
         <v>114</v>
       </c>
       <c r="J37" t="s">
-        <v>138</v>
-      </c>
-      <c r="K37" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B38" s="9"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="10"/>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F38" s="4">
         <v>43663</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="H38" s="4">
         <v>43663</v>
       </c>
       <c r="I38" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="J38" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B39" s="9"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="10"/>
       <c r="C39" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E39" t="s">
         <v>37</v>
@@ -2041,328 +2043,381 @@
         <v>43663</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H39" s="4">
         <v>43663</v>
       </c>
       <c r="I39" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J39" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B40" s="9"/>
+        <v>135</v>
+      </c>
+      <c r="K39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="10"/>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="4">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="H40" s="4">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="I40" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B41" s="9"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="10"/>
       <c r="C41" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F41" s="4">
         <v>43664</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="H41" s="4">
         <v>43664</v>
       </c>
       <c r="I41" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="J41" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="10"/>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="4">
+        <v>43664</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" s="4">
+        <v>43664</v>
+      </c>
+      <c r="I42" t="s">
+        <v>103</v>
+      </c>
+      <c r="J42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>41</v>
       </c>
-      <c r="D42" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42" t="s">
-        <v>89</v>
-      </c>
-      <c r="F42" s="4">
-        <v>43669</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B43" s="6"/>
-      <c r="C43" t="s">
-        <v>63</v>
-      </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E43" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F43" s="4">
         <v>43669</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B44" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="6"/>
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" s="4">
+        <v>43669</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B45" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C44" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" t="s">
-        <v>84</v>
-      </c>
-      <c r="E44" t="s">
-        <v>91</v>
-      </c>
-      <c r="F44" s="4">
-        <v>43670</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F45" s="4">
         <v>43670</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B46" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>70</v>
+        <v>90</v>
+      </c>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="7"/>
+      <c r="C46" t="s">
+        <v>64</v>
       </c>
       <c r="D46" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F46" s="4">
         <v>43670</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B47" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="C47" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E47" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F47" s="4">
         <v>43670</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B48" s="7"/>
       <c r="C48" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F48" s="4">
         <v>43670</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="33" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B49" s="7"/>
       <c r="C49" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E49" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F49" s="4">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B50" s="7"/>
       <c r="C50" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E50" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F50" s="4">
         <v>43671</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="7"/>
       <c r="C51" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F51" s="4">
         <v>43671</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="7"/>
       <c r="C52" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E52" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F52" s="4">
         <v>43671</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="7"/>
+      <c r="C53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="4">
+        <v>43671</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
         <v>108</v>
       </c>
-      <c r="C53" t="s">
-        <v>109</v>
-      </c>
-      <c r="D53" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" t="s">
-        <v>112</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="F54" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="7"/>
+      <c r="C55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" t="s">
         <v>9</v>
       </c>
-      <c r="E54" t="s">
-        <v>112</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
+        <v>108</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="7"/>
+      <c r="C56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" t="s">
         <v>7</v>
       </c>
-      <c r="E55" t="s">
-        <v>112</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G55" s="2" t="s">
+      <c r="E56" t="s">
+        <v>108</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="H56" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B35:B41"/>
+    <mergeCell ref="B36:B42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Goods-Controller Test (고객 상품관련 완료) _ API Ver 1.6
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B56466FC-2AA0-4965-B198-40B9A7939CBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7534ED40-D000-4907-85A2-C332A9200B47}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -16,18 +16,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="170">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,10 +211,6 @@
   </si>
   <si>
     <t>장바구니상품삭제 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품상세조회API -</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -730,30 +720,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관리자 상품등록 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 상품수정 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 상품삭제 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 상품상세조회 API - (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>보류- 상품수정시 함께?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관리자 상품리스트조회 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상품옵션 수정불가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -774,34 +744,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상품검색 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/goods/view/{goodsNo}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상품상세옵션리스트조회 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/goods/goodsdetail/{goodsNo}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상품서브이미지리스트조회 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/goods/subimagelist/{goodsNo}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상품 메인이미지 조회 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/goods/mainimage/{goodsNo}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -854,7 +808,242 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API</t>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88%EB%93%B1%EB%A1%9D-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">관리자 상품등록 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">관리자 상품리스트조회 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">관리자 상품상세조회 API - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88%EB%A6%AC%EC%8A%A4%ED%8A%B8%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88%EC%83%81%EC%84%B8%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">관리자 상품수정 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88%EC%88%98%EC%A0%95-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">관리자 상품삭제 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88%EC%82%AD%EC%A0%9C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EC%83%81%ED%92%88%EA%B2%80%EC%83%89-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">상품검색 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EC%83%81%ED%92%88%EC%83%81%EC%84%B8%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">상품상세조회API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EC%83%81%ED%92%88-%EB%A9%94%EC%9D%B8%EC%9D%B4%EB%AF%B8%EC%A7%80-%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">상품 메인이미지 조회 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">상품서브이미지리스트조회 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EC%83%81%ED%92%88%EC%84%9C%EB%B8%8C%EC%9D%B4%EB%AF%B8%EC%A7%80%EB%A6%AC%EC%8A%A4%ED%8A%B8%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">상품상세옵션리스트조회 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%EC%83%81%ED%92%88%EC%83%81%EC%84%B8%EC%98%B5%EC%85%98%EB%A6%AC%EC%8A%A4%ED%8A%B8%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5H</t>
+  </si>
+  <si>
+    <t>0.5H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.3H</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -924,12 +1113,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -943,6 +1126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -989,9 +1178,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1001,26 +1187,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1339,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
   <dimension ref="A2:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1352,7 +1541,7 @@
     <col min="6" max="6" width="10.625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="234.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="48.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1388,7 +1577,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
@@ -1399,7 +1588,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -1407,7 +1596,7 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <v>43662</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1417,15 +1606,15 @@
         <v>43662</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J3" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1433,7 +1622,7 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="14">
         <v>43662</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1443,41 +1632,41 @@
         <v>43662</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="17">
+        <v>97</v>
+      </c>
+      <c r="F5" s="14">
         <v>43662</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="4">
         <v>43662</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J5" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1485,7 +1674,7 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="14">
         <v>43662</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1495,15 +1684,15 @@
         <v>43662</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J6" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1511,7 +1700,7 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <v>43662</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1521,15 +1710,15 @@
         <v>43662</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1537,81 +1726,81 @@
       <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <v>43662</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="4">
         <v>43662</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J8" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="5"/>
       <c r="G12" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
@@ -1623,16 +1812,16 @@
       <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="12">
         <v>43669</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="18"/>
       <c r="C14" t="s">
         <v>43</v>
       </c>
@@ -1642,15 +1831,15 @@
       <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <v>43669</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="18"/>
       <c r="C15" t="s">
         <v>44</v>
       </c>
@@ -1664,11 +1853,11 @@
         <v>43670</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
+      <c r="B16" s="18"/>
       <c r="C16" t="s">
         <v>45</v>
       </c>
@@ -1682,15 +1871,15 @@
         <v>43670</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1698,182 +1887,235 @@
       <c r="E17" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="13">
         <v>43665</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>88</v>
+        <v>166</v>
+      </c>
+      <c r="H17" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I17" t="s">
+        <v>166</v>
+      </c>
+      <c r="J17" t="s">
+        <v>156</v>
       </c>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
+      <c r="B18" s="10"/>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
-      </c>
-      <c r="F18" s="8">
+        <v>129</v>
+      </c>
+      <c r="F18" s="13">
         <v>43665</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="H18" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J18" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11"/>
+      <c r="B19" s="10"/>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="4"/>
+        <v>132</v>
+      </c>
+      <c r="F19" s="13">
+        <v>43665</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I19" t="s">
+        <v>169</v>
+      </c>
+      <c r="J19" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="11"/>
+      <c r="B20" s="10"/>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="4"/>
+        <v>131</v>
+      </c>
+      <c r="F20" s="13">
+        <v>43665</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I20" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="11"/>
+      <c r="B21" s="10"/>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="4"/>
+        <v>130</v>
+      </c>
+      <c r="F21" s="13">
+        <v>43665</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H21" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I21" t="s">
+        <v>169</v>
+      </c>
+      <c r="J21" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="22" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
         <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="8">
+        <v>73</v>
+      </c>
+      <c r="F22" s="16">
         <v>43668</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="8">
+        <v>73</v>
+      </c>
+      <c r="F23" s="16">
         <v>43668</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="8">
+        <v>73</v>
+      </c>
+      <c r="F24" s="16">
         <v>43668</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="15">
+        <v>79</v>
+      </c>
+      <c r="F25" s="12">
         <v>43669</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="15">
+        <v>79</v>
+      </c>
+      <c r="F26" s="12">
         <v>43669</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="15">
+        <v>79</v>
+      </c>
+      <c r="F27" s="12">
         <v>43669</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H27" s="4"/>
     </row>
@@ -1885,7 +2127,7 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
         <v>24</v>
@@ -1893,18 +2135,26 @@
       <c r="E28" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="13">
         <v>43665</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H28" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="H28" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I28" t="s">
+        <v>166</v>
+      </c>
+      <c r="J28" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="9"/>
+      <c r="B29" s="8"/>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1912,18 +2162,26 @@
       <c r="E29" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="13">
         <v>43665</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H29" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="H29" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I29" t="s">
+        <v>166</v>
+      </c>
+      <c r="J29" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="D30" t="s">
         <v>25</v>
@@ -1931,18 +2189,26 @@
       <c r="E30" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="13">
         <v>43665</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H30" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="H30" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I30" t="s">
+        <v>168</v>
+      </c>
+      <c r="J30" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6"/>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
@@ -1950,18 +2216,26 @@
       <c r="E31" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="13">
         <v>43665</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H31" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="H31" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I31" t="s">
+        <v>168</v>
+      </c>
+      <c r="J31" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D32" t="s">
         <v>27</v>
@@ -1969,146 +2243,154 @@
       <c r="E32" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="13">
         <v>43665</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H32" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="H32" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I32" t="s">
+        <v>168</v>
+      </c>
+      <c r="J32" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="12" t="s">
-        <v>117</v>
+      <c r="B33" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F33" s="4">
         <v>43668</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="12" t="s">
-        <v>128</v>
+      <c r="B34" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F34" s="4">
         <v>43668</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="12" t="s">
-        <v>133</v>
+      <c r="B35" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F35" s="4">
         <v>43668</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="12" t="s">
-        <v>131</v>
+      <c r="B36" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F36" s="4">
         <v>43668</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="12" t="s">
-        <v>130</v>
+      <c r="B37" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F37" s="4">
         <v>43668</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="4">
+        <v>81</v>
+      </c>
+      <c r="F38" s="16">
         <v>43668</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
         <v>24</v>
@@ -2116,29 +2398,29 @@
       <c r="E39" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="13">
         <v>43663</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H39" s="4">
         <v>43663</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="K39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="13"/>
+      <c r="B40" s="17"/>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
         <v>26</v>
@@ -2146,26 +2428,26 @@
       <c r="E40" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F40" s="13">
         <v>43663</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H40" s="4">
         <v>43663</v>
       </c>
       <c r="I40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J40" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="13"/>
+      <c r="B41" s="17"/>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D41" t="s">
         <v>27</v>
@@ -2173,29 +2455,29 @@
       <c r="E41" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="16">
+      <c r="F41" s="13">
         <v>43663</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H41" s="4">
         <v>43663</v>
       </c>
       <c r="I41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J41" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="K41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="13"/>
+      <c r="B42" s="17"/>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42" t="s">
         <v>24</v>
@@ -2203,29 +2485,29 @@
       <c r="E42" t="s">
         <v>36</v>
       </c>
-      <c r="F42" s="16">
+      <c r="F42" s="13">
         <v>43663</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H42" s="4">
         <v>43663</v>
       </c>
       <c r="I42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J42" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="K42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="13"/>
+      <c r="B43" s="17"/>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D43" t="s">
         <v>26</v>
@@ -2233,26 +2515,26 @@
       <c r="E43" t="s">
         <v>36</v>
       </c>
-      <c r="F43" s="16">
+      <c r="F43" s="13">
         <v>43663</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H43" s="4">
         <v>43663</v>
       </c>
       <c r="I43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J43" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="13"/>
+      <c r="B44" s="17"/>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
@@ -2260,26 +2542,26 @@
       <c r="E44" t="s">
         <v>36</v>
       </c>
-      <c r="F44" s="16">
+      <c r="F44" s="13">
         <v>43664</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H44" s="4">
         <v>43664</v>
       </c>
       <c r="I44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J44" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="13"/>
+      <c r="B45" s="17"/>
       <c r="C45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D45" t="s">
         <v>25</v>
@@ -2287,20 +2569,20 @@
       <c r="E45" t="s">
         <v>37</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="13">
         <v>43664</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H45" s="4">
         <v>43664</v>
       </c>
       <c r="I45" t="s">
-        <v>101</v>
-      </c>
-      <c r="J45" s="18" t="s">
-        <v>155</v>
+        <v>100</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -2311,35 +2593,35 @@
         <v>40</v>
       </c>
       <c r="D46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F46" s="4">
         <v>43669</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6"/>
       <c r="C47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F47" s="4">
         <v>43669</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H47" s="4"/>
     </row>
@@ -2348,229 +2630,229 @@
         <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F48" s="4">
         <v>43670</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F49" s="4">
         <v>43670</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F50" s="4">
         <v>43670</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B51" s="7"/>
       <c r="C51" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="4">
         <v>43670</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B52" s="7"/>
       <c r="C52" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F52" s="4">
         <v>43670</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
       <c r="C53" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F53" s="4">
         <v>43671</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
       <c r="C54" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F54" s="4">
         <v>43671</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
       <c r="C55" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F55" s="4">
         <v>43671</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F56" s="4">
         <v>43671</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" t="s">
         <v>102</v>
-      </c>
-      <c r="C57" t="s">
-        <v>103</v>
       </c>
       <c r="D57" t="s">
         <v>4</v>
       </c>
       <c r="E57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
       <c r="C59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>34</v>
@@ -2584,7 +2866,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J45" r:id="rId1" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
+    <hyperlink ref="J45" r:id="rId1" display="https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
success message 변경 및 API 일정문서 수정
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4F582BBF-CEE3-4BA6-BA8D-BE793482C355}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EEADAA2E-1439-470F-8B26-6D356CE64CB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="180">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1043,14 +1043,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>주문 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문코드에 따른 상품상세조회 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1H</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1059,15 +1051,95 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>주문코드에 따른 주문자정보 및 배송지정보 조회 API (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/order/cancel</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>주문취소 API (완)</t>
+    <t>[링크](https://github.com/skok1025/ShoppingMall_backend/wiki/%EC%A3%BC%EB%AC%B8-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall_backend/wiki/%EC%A3%BC%EB%AC%B8%EC%BD%94%EB%93%9C%EC%97%90-%EB%94%B0%EB%A5%B8-%EC%83%81%ED%92%88%EC%83%81%EC%84%B8%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall_backend/wiki/%EC%A3%BC%EB%AC%B8%EC%BD%94%EB%93%9C%EC%97%90-%EB%94%B0%EB%A5%B8-%EC%A3%BC%EB%AC%B8%EC%9E%90%EC%A0%95%EB%B3%B4-%EB%B0%8F-%EB%B0%B0%EC%86%A1%EC%A7%80%EC%A0%95%EB%B3%B4-%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall_backend/wiki/%EC%A3%BC%EB%AC%B8%EC%B7%A8%EC%86%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">주문 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">주문코드에 따른 상품상세조회 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">주문코드에 따른 주문자정보 및 배송지정보 조회 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">주문취소 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1555,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
   <dimension ref="A2:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2035,7 +2107,7 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -2043,23 +2115,26 @@
       <c r="E22" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="13">
         <v>43668</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H22" s="4">
         <v>43668</v>
       </c>
       <c r="I22" t="s">
-        <v>171</v>
+        <v>85</v>
+      </c>
+      <c r="J22" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="17"/>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -2067,7 +2142,7 @@
       <c r="E23" t="s">
         <v>167</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="13">
         <v>43668</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -2077,13 +2152,16 @@
         <v>43668</v>
       </c>
       <c r="I23" t="s">
-        <v>172</v>
+        <v>170</v>
+      </c>
+      <c r="J23" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -2091,7 +2169,7 @@
       <c r="E24" t="s">
         <v>168</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="13">
         <v>43668</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2101,27 +2179,33 @@
         <v>43668</v>
       </c>
       <c r="I24" t="s">
-        <v>171</v>
+        <v>169</v>
+      </c>
+      <c r="J24" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" s="16">
+        <v>171</v>
+      </c>
+      <c r="F25" s="13">
         <v>43668</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>84</v>
       </c>
       <c r="H25" s="4"/>
+      <c r="J25" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>

</xml_diff>

<commit_message>
Order-Controller Test (주문관련 완료) _ API Ver 1.8
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EEADAA2E-1439-470F-8B26-6D356CE64CB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{332C505D-FA94-402F-9BB4-6D932721534F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="194">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -301,18 +301,6 @@
   </si>
   <si>
     <t>관리자 상품 메인진열 삭제 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 교환신청 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 교환신청내역조회 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문 교환신청 취소 API</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1127,6 +1115,131 @@
   <si>
     <r>
       <t xml:space="preserve">주문취소 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/order/change/{orderCode}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문코드 unique 제약 및 
+주문코드 날짜별 order 생성 ex) 20190723-00001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/order/goodslist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문서작업 (API 작성 고민거리) 으로 인한 시작지연 +2H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API 수정작업 (상품등록 연쇄적인 insert를위한 last_insert_id 사용 ) +2H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%A3%BC%EB%AC%B8-%EA%B5%90%ED%99%98%EC%8B%A0%EC%B2%AD-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">주문 교환신청 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">주문 교환신청내역조회 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%A3%BC%EB%AC%B8-%EA%B5%90%ED%99%98%EC%8B%A0%EC%B2%AD%EB%82%B4%EC%97%AD%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%A3%BC%EB%AC%B8-%EA%B5%90%ED%99%98%EC%8B%A0%EC%B2%AD-%EC%B7%A8%EC%86%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%ED%9A%8C%EC%9B%90-%EC%A3%BC%EB%AC%B8%EB%82%B4%EC%97%AD-%EC%A1%B0%ED%9A%8C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">주문 교환신청 취소 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">회원 주문 내역 조회 API </t>
     </r>
     <r>
       <rPr>
@@ -1249,7 +1362,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1300,6 +1413,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1625,17 +1741,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
-  <dimension ref="A2:K60"/>
+  <dimension ref="A2:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.25" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
@@ -1676,7 +1792,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
@@ -1687,7 +1803,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -1705,15 +1821,15 @@
         <v>43662</v>
       </c>
       <c r="I3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1731,41 +1847,41 @@
         <v>43662</v>
       </c>
       <c r="I4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" s="14">
         <v>43662</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H5" s="4">
         <v>43662</v>
       </c>
       <c r="I5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1783,15 +1899,15 @@
         <v>43662</v>
       </c>
       <c r="I6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1809,15 +1925,15 @@
         <v>43662</v>
       </c>
       <c r="I7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1829,16 +1945,16 @@
         <v>43662</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H8" s="4">
         <v>43662</v>
       </c>
       <c r="I8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1849,13 +1965,13 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1866,13 +1982,13 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1883,23 +1999,23 @@
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="5"/>
       <c r="G12" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
@@ -1915,12 +2031,12 @@
         <v>43669</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="19"/>
+      <c r="B14" s="20"/>
       <c r="C14" t="s">
         <v>43</v>
       </c>
@@ -1934,11 +2050,11 @@
         <v>43669</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="19"/>
+      <c r="B15" s="20"/>
       <c r="C15" t="s">
         <v>44</v>
       </c>
@@ -1952,11 +2068,11 @@
         <v>43670</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
+      <c r="B16" s="20"/>
       <c r="C16" t="s">
         <v>45</v>
       </c>
@@ -1970,7 +2086,7 @@
         <v>43670</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.3">
@@ -1978,7 +2094,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -1990,116 +2106,116 @@
         <v>43665</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H17" s="4">
         <v>43665</v>
       </c>
       <c r="I17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F18" s="13">
         <v>43665</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H18" s="4">
         <v>43665</v>
       </c>
       <c r="I18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F19" s="13">
         <v>43665</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H19" s="4">
         <v>43665</v>
       </c>
       <c r="I19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F20" s="13">
         <v>43665</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H20" s="4">
         <v>43665</v>
       </c>
       <c r="I20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J20" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F21" s="13">
         <v>43665</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H21" s="4">
         <v>43665</v>
       </c>
       <c r="I21" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -2107,256 +2223,294 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F22" s="13">
         <v>43668</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H22" s="4">
         <v>43668</v>
       </c>
       <c r="I22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J22" t="s">
-        <v>172</v>
+        <v>169</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="17"/>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="F23" s="13">
         <v>43668</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H23" s="4">
         <v>43668</v>
       </c>
       <c r="I23" t="s">
+        <v>167</v>
+      </c>
+      <c r="J23" t="s">
         <v>170</v>
-      </c>
-      <c r="J23" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F24" s="13">
         <v>43668</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H24" s="4">
         <v>43668</v>
       </c>
       <c r="I24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F25" s="13">
         <v>43668</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="H25" s="4">
+        <v>43668</v>
+      </c>
+      <c r="I25" t="s">
+        <v>180</v>
+      </c>
       <c r="J25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>187</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="12">
+        <v>73</v>
+      </c>
+      <c r="F26" s="13">
         <v>43669</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="H26" s="4">
+        <v>43669</v>
+      </c>
+      <c r="I26" t="s">
+        <v>180</v>
+      </c>
+      <c r="J26" t="s">
+        <v>186</v>
+      </c>
+      <c r="K26" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>188</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="12">
+        <v>177</v>
+      </c>
+      <c r="F27" s="13">
         <v>43669</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="H27" s="4">
+        <v>43669</v>
+      </c>
+      <c r="I27" t="s">
+        <v>181</v>
+      </c>
+      <c r="J27" t="s">
+        <v>189</v>
+      </c>
+      <c r="K27" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="7"/>
+      <c r="B28" s="18"/>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>192</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="12">
+        <v>73</v>
+      </c>
+      <c r="F28" s="13">
         <v>43669</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+        <v>184</v>
+      </c>
+      <c r="H28" s="4">
+        <v>43670</v>
+      </c>
+      <c r="I28" t="s">
+        <v>184</v>
+      </c>
+      <c r="J28" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="7"/>
+      <c r="C29" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="13">
+        <v>43669</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H29" s="4">
+        <v>43670</v>
+      </c>
+      <c r="I29" t="s">
+        <v>185</v>
+      </c>
+      <c r="J29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" t="s">
         <v>24</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>38</v>
-      </c>
-      <c r="F29" s="13">
-        <v>43665</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H29" s="4">
-        <v>43665</v>
-      </c>
-      <c r="I29" t="s">
-        <v>163</v>
-      </c>
-      <c r="J29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="8"/>
-      <c r="C30" t="s">
-        <v>145</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" t="s">
-        <v>39</v>
       </c>
       <c r="F30" s="13">
         <v>43665</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H30" s="4">
         <v>43665</v>
       </c>
       <c r="I30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J30" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="6"/>
+      <c r="B31" s="8"/>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F31" s="13">
         <v>43665</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H31" s="4">
         <v>43665</v>
       </c>
       <c r="I31" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="J31" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
         <v>38</v>
@@ -2365,25 +2519,25 @@
         <v>43665</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H32" s="4">
         <v>43665</v>
       </c>
       <c r="I32" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J32" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
         <v>38</v>
@@ -2392,183 +2546,180 @@
         <v>43665</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H33" s="4">
         <v>43665</v>
       </c>
       <c r="I33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J33" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="11" t="s">
-        <v>113</v>
-      </c>
+      <c r="B34" s="6"/>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>77</v>
-      </c>
-      <c r="F34" s="4">
-        <v>43668</v>
+        <v>38</v>
+      </c>
+      <c r="F34" s="13">
+        <v>43665</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H34" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="H34" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I34" t="s">
+        <v>162</v>
+      </c>
+      <c r="J34" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="11" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F35" s="4">
         <v>43668</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F36" s="4">
         <v>43668</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F37" s="4">
         <v>43668</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F38" s="4">
         <v>43668</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B39" s="6" t="s">
-        <v>123</v>
+    <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
+        <v>118</v>
       </c>
       <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" s="4">
+        <v>43668</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B40" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
         <v>52</v>
       </c>
-      <c r="D39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F39" s="16">
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40" s="16">
         <v>43668</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="18" t="s">
+      <c r="G40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C40" t="s">
-        <v>103</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
         <v>24</v>
-      </c>
-      <c r="E40" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="13">
-        <v>43663</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H40" s="4">
-        <v>43663</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K40" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="18"/>
-      <c r="C41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" t="s">
-        <v>26</v>
       </c>
       <c r="E41" t="s">
         <v>35</v>
@@ -2577,25 +2728,28 @@
         <v>43663</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="H41" s="4">
         <v>43663</v>
       </c>
-      <c r="I41" t="s">
-        <v>108</v>
-      </c>
-      <c r="J41" t="s">
-        <v>137</v>
+      <c r="I41" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K41" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="18"/>
+      <c r="B42" s="19"/>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E42" t="s">
         <v>35</v>
@@ -2604,58 +2758,55 @@
         <v>43663</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="H42" s="4">
         <v>43663</v>
       </c>
       <c r="I42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J42" t="s">
-        <v>138</v>
-      </c>
-      <c r="K42" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="18"/>
+      <c r="B43" s="19"/>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" s="13">
         <v>43663</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="H43" s="4">
         <v>43663</v>
       </c>
       <c r="I43" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="J43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K43" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="18"/>
+      <c r="B44" s="19"/>
       <c r="C44" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E44" t="s">
         <v>36</v>
@@ -2664,354 +2815,384 @@
         <v>43663</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H44" s="4">
         <v>43663</v>
       </c>
       <c r="I44" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J44" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="K44" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="18"/>
+      <c r="B45" s="19"/>
       <c r="C45" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
         <v>36</v>
       </c>
       <c r="F45" s="13">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H45" s="4">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="I45" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J45" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="18"/>
+      <c r="B46" s="19"/>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F46" s="13">
         <v>43664</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="H46" s="4">
         <v>43664</v>
       </c>
       <c r="I46" t="s">
-        <v>97</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B47" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J46" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="19"/>
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="13">
+        <v>43664</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H47" s="4">
+        <v>43664</v>
+      </c>
+      <c r="I47" t="s">
+        <v>94</v>
+      </c>
+      <c r="J47" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B48" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>40</v>
       </c>
-      <c r="D47" t="s">
-        <v>74</v>
-      </c>
-      <c r="E47" t="s">
-        <v>79</v>
-      </c>
-      <c r="F47" s="4">
-        <v>43669</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="6"/>
-      <c r="C48" t="s">
-        <v>53</v>
-      </c>
       <c r="D48" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F48" s="4">
         <v>43669</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B49" s="6" t="s">
+    <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="6"/>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="4">
+        <v>43669</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B50" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>57</v>
       </c>
-      <c r="D49" t="s">
-        <v>74</v>
-      </c>
-      <c r="E49" t="s">
-        <v>81</v>
-      </c>
-      <c r="F49" s="4">
-        <v>43670</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="7"/>
-      <c r="C50" t="s">
-        <v>58</v>
-      </c>
       <c r="D50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F50" s="4">
         <v>43670</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B51" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>60</v>
+    <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="7"/>
+      <c r="C51" t="s">
+        <v>58</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F51" s="4">
         <v>43670</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B52" s="7"/>
+      <c r="B52" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="C52" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F52" s="4">
         <v>43670</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
       <c r="C53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
         <v>71</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F53" s="4">
         <v>43670</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
       <c r="C54" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F54" s="4">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
       <c r="C55" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F55" s="4">
         <v>43671</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E56" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F56" s="4">
         <v>43671</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="7"/>
       <c r="C57" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F57" s="4">
         <v>43671</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B58" s="7"/>
+      <c r="C58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" s="4">
+        <v>43671</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
         <v>99</v>
       </c>
-      <c r="D58" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" t="s">
-        <v>102</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="7"/>
-      <c r="C59" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" t="s">
-        <v>102</v>
-      </c>
       <c r="F59" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>99</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="7"/>
+      <c r="C61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" t="s">
         <v>7</v>
       </c>
-      <c r="E60" t="s">
-        <v>102</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G60" s="2" t="s">
+      <c r="E61" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H60" s="4"/>
+      <c r="H61" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="B41:B47"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J46" r:id="rId1" display="https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
+    <hyperlink ref="J47" r:id="rId1" display="https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
frontend css, js 세팅
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{332C505D-FA94-402F-9BB4-6D932721534F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7F1E3AAE-931E-425F-B9B4-B5E9807CEA71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -736,10 +736,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/1.-%ED%9A%8C%EC%9B%90%EA%B0%80%EC%9E%85-API)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[링크](https://github.com/skok1025/ShoppingMall-2week-/wiki/%ED%9A%8C%EC%9B%90%EC%A0%95%EB%B3%B4-%EC%88%98%EC%A0%95-API)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1253,6 +1249,10 @@
       </rPr>
       <t>(완)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%ED%9A%8C%EC%9B%90%EA%B0%80%EC%9E%85-API)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1743,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
   <dimension ref="A2:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1824,7 +1824,7 @@
         <v>87</v>
       </c>
       <c r="J3" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1850,7 +1850,7 @@
         <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1876,7 +1876,7 @@
         <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1902,7 +1902,7 @@
         <v>94</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1928,7 +1928,7 @@
         <v>89</v>
       </c>
       <c r="J7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1954,7 +1954,7 @@
         <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2094,7 +2094,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -2106,23 +2106,23 @@
         <v>43665</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H17" s="4">
         <v>43665</v>
       </c>
       <c r="I17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -2134,22 +2134,22 @@
         <v>43665</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H18" s="4">
         <v>43665</v>
       </c>
       <c r="I18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
         <v>126</v>
@@ -2158,22 +2158,22 @@
         <v>43665</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H19" s="4">
         <v>43665</v>
       </c>
       <c r="I19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
         <v>125</v>
@@ -2182,22 +2182,22 @@
         <v>43665</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H20" s="4">
         <v>43665</v>
       </c>
       <c r="I20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
         <v>124</v>
@@ -2206,16 +2206,16 @@
         <v>43665</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H21" s="4">
         <v>43665</v>
       </c>
       <c r="I21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -2223,7 +2223,7 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -2235,7 +2235,7 @@
         <v>43668</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H22" s="4">
         <v>43668</v>
@@ -2244,22 +2244,22 @@
         <v>82</v>
       </c>
       <c r="J22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="17"/>
       <c r="C23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F23" s="13">
         <v>43668</v>
@@ -2271,22 +2271,22 @@
         <v>43668</v>
       </c>
       <c r="I23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F24" s="13">
         <v>43668</v>
@@ -2298,22 +2298,22 @@
         <v>43668</v>
       </c>
       <c r="I24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F25" s="13">
         <v>43668</v>
@@ -2325,16 +2325,16 @@
         <v>43668</v>
       </c>
       <c r="I25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
@@ -2352,25 +2352,25 @@
         <v>43669</v>
       </c>
       <c r="I26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F27" s="13">
         <v>43669</v>
@@ -2382,19 +2382,19 @@
         <v>43669</v>
       </c>
       <c r="I27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="18"/>
       <c r="C28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -2406,28 +2406,28 @@
         <v>43669</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H28" s="4">
         <v>43670</v>
       </c>
       <c r="I28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F29" s="13">
         <v>43669</v>
@@ -2439,10 +2439,10 @@
         <v>43670</v>
       </c>
       <c r="I29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -2453,7 +2453,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
         <v>24</v>
@@ -2471,16 +2471,16 @@
         <v>43665</v>
       </c>
       <c r="I30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
       <c r="C31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -2498,16 +2498,16 @@
         <v>43665</v>
       </c>
       <c r="I31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
       <c r="C32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D32" t="s">
         <v>25</v>
@@ -2525,16 +2525,16 @@
         <v>43665</v>
       </c>
       <c r="I32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
         <v>26</v>
@@ -2552,16 +2552,16 @@
         <v>43665</v>
       </c>
       <c r="I33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -2579,10 +2579,10 @@
         <v>43665</v>
       </c>
       <c r="I34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
@@ -2737,7 +2737,7 @@
         <v>102</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K41" t="s">
         <v>104</v>
@@ -2767,7 +2767,7 @@
         <v>105</v>
       </c>
       <c r="J42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
@@ -2794,7 +2794,7 @@
         <v>101</v>
       </c>
       <c r="J43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K43" t="s">
         <v>107</v>
@@ -2824,7 +2824,7 @@
         <v>105</v>
       </c>
       <c r="J44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K44" t="s">
         <v>112</v>
@@ -2854,7 +2854,7 @@
         <v>105</v>
       </c>
       <c r="J45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
@@ -2881,7 +2881,7 @@
         <v>105</v>
       </c>
       <c r="J46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
@@ -2908,7 +2908,7 @@
         <v>94</v>
       </c>
       <c r="J47" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Basket-Controller Test (장바구니관련 부분완료 ~ 장바구니조회 (비회원)) _ API Ver 1.9
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{588C7440-2335-4F25-ADFE-C1C99682659C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4022C912-52FB-47C1-9605-4D623E59B7C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="199">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,14 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/api/basket/add/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/basket/list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/basket/modify</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,14 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니추가 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니조회 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>장바구니수정 API -</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1220,6 +1204,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>/api/basket/member/add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/basket/nonmember/add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니추가 API (회원) (완)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니추가 API (비회원) (완)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">프론트엔드 테마작업 및 부분 템플릿화(header,footer) +4H </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">회원가입 API </t>
     </r>
@@ -1234,6 +1238,17 @@
         <scheme val="minor"/>
       </rPr>
       <t>(완) - 수정 : 장바구니코드 배정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 7/25 + 1H</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1263,8 +1278,48 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - 수정 : 비회원 장바구니 등록 후, 로그인 후 장바구니 상품 유지</t>
-    </r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- 수정 : 비회원 장바구니 등록 후, 로그인 후 장바구니 상품 유지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+7/25 + 1H</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니조회 API (회원)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/basket/member/list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/basket/nonmember/list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니조회 API (비회원) (완)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1374,7 +1429,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1434,9 +1489,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1753,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
-  <dimension ref="A2:K61"/>
+  <dimension ref="A2:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1789,33 +1841,33 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -1827,21 +1879,21 @@
         <v>43662</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3" s="4">
         <v>43662</v>
       </c>
       <c r="I3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1853,47 +1905,47 @@
         <v>43662</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" s="4">
         <v>43662</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F5" s="14">
         <v>43662</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H5" s="4">
         <v>43662</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1905,21 +1957,21 @@
         <v>43662</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H6" s="4">
         <v>43662</v>
       </c>
       <c r="I6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1931,1280 +1983,1324 @@
         <v>43662</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7" s="4">
         <v>43662</v>
       </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="14">
         <v>43662</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H8" s="4">
         <v>43662</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="5"/>
       <c r="G12" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
-        <v>17</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>188</v>
       </c>
       <c r="F13" s="12">
         <v>43669</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
+        <v>77</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="K13" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>189</v>
       </c>
       <c r="F14" s="12">
         <v>43669</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
+        <v>77</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>195</v>
       </c>
       <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>196</v>
+      </c>
+      <c r="F15" s="12">
+        <v>43669</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16" s="12">
+        <v>43669</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="4">
         <v>43670</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="G17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="4">
+        <v>43670</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
         <v>16</v>
-      </c>
-      <c r="F16" s="4">
-        <v>43670</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="13">
-        <v>43665</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H17" s="4">
-        <v>43665</v>
-      </c>
-      <c r="I17" t="s">
-        <v>157</v>
-      </c>
-      <c r="J17" t="s">
-        <v>147</v>
-      </c>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>121</v>
-      </c>
-      <c r="F18" s="13">
-        <v>43665</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H18" s="4">
-        <v>43665</v>
-      </c>
-      <c r="I18" t="s">
-        <v>159</v>
-      </c>
-      <c r="J18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" t="s">
-        <v>124</v>
       </c>
       <c r="F19" s="13">
         <v>43665</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H19" s="4">
         <v>43665</v>
       </c>
       <c r="I19" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="J19" t="s">
-        <v>151</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="10"/>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>146</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F20" s="13">
         <v>43665</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H20" s="4">
         <v>43665</v>
       </c>
       <c r="I20" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="J20" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F21" s="13">
         <v>43665</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H21" s="4">
         <v>43665</v>
       </c>
       <c r="I21" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="13">
+        <v>43665</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H22" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I22" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="13">
-        <v>43668</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H22" s="4">
-        <v>43668</v>
-      </c>
-      <c r="I22" t="s">
-        <v>82</v>
-      </c>
       <c r="J22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="10"/>
+      <c r="C23" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="13">
+        <v>43665</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I23" t="s">
+        <v>156</v>
+      </c>
+      <c r="J23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
         <v>166</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
-      <c r="C23" t="s">
-        <v>171</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="13">
-        <v>43668</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="4">
-        <v>43668</v>
-      </c>
-      <c r="I23" t="s">
-        <v>164</v>
-      </c>
-      <c r="J23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
-      <c r="C24" t="s">
-        <v>172</v>
-      </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>162</v>
+        <v>63</v>
       </c>
       <c r="F24" s="13">
         <v>43668</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>81</v>
+        <v>159</v>
       </c>
       <c r="H24" s="4">
         <v>43668</v>
       </c>
       <c r="I24" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="J24" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
+      <c r="B25" s="17"/>
       <c r="C25" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F25" s="13">
         <v>43668</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H25" s="4">
         <v>43668</v>
       </c>
       <c r="I25" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="J25" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="F26" s="13">
-        <v>43669</v>
+        <v>43668</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H26" s="4">
-        <v>43669</v>
+        <v>43668</v>
       </c>
       <c r="I26" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="J26" t="s">
-        <v>183</v>
-      </c>
-      <c r="K26" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="F27" s="13">
-        <v>43669</v>
+        <v>43668</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H27" s="4">
-        <v>43669</v>
+        <v>43668</v>
       </c>
       <c r="I27" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J27" t="s">
-        <v>186</v>
-      </c>
-      <c r="K27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7"/>
+      <c r="C28" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="18"/>
-      <c r="C28" t="s">
-        <v>189</v>
-      </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F28" s="13">
         <v>43669</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>181</v>
+        <v>77</v>
       </c>
       <c r="H28" s="4">
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="I28" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="J28" t="s">
-        <v>187</v>
+        <v>179</v>
+      </c>
+      <c r="K28" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="F29" s="13">
         <v>43669</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H29" s="4">
+        <v>43669</v>
+      </c>
+      <c r="I29" t="s">
+        <v>174</v>
+      </c>
+      <c r="J29" t="s">
+        <v>182</v>
+      </c>
+      <c r="K29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="18"/>
+      <c r="C30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="13">
+        <v>43669</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" s="4">
         <v>43670</v>
       </c>
-      <c r="I29" t="s">
-        <v>182</v>
-      </c>
-      <c r="J29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="13">
-        <v>43665</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H30" s="4">
-        <v>43665</v>
-      </c>
       <c r="I30" t="s">
+        <v>177</v>
+      </c>
+      <c r="J30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7"/>
+      <c r="C31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
         <v>157</v>
       </c>
-      <c r="J30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="8"/>
-      <c r="C31" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>39</v>
-      </c>
       <c r="F31" s="13">
-        <v>43665</v>
+        <v>43669</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H31" s="4">
-        <v>43665</v>
+        <v>43670</v>
       </c>
       <c r="I31" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="J31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="6"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F32" s="13">
         <v>43665</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H32" s="4">
         <v>43665</v>
       </c>
       <c r="I32" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J32" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="6"/>
+      <c r="B33" s="8"/>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F33" s="13">
         <v>43665</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H33" s="4">
         <v>43665</v>
       </c>
       <c r="I33" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J33" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F34" s="13">
         <v>43665</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H34" s="4">
         <v>43665</v>
       </c>
       <c r="I34" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J34" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="11" t="s">
-        <v>108</v>
-      </c>
+      <c r="B35" s="6"/>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="4">
-        <v>43668</v>
+        <v>36</v>
+      </c>
+      <c r="F35" s="13">
+        <v>43665</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H35" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="H35" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I35" t="s">
+        <v>155</v>
+      </c>
+      <c r="J35" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="11" t="s">
-        <v>115</v>
-      </c>
+      <c r="B36" s="6"/>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="4">
-        <v>43668</v>
+        <v>36</v>
+      </c>
+      <c r="F36" s="13">
+        <v>43665</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H36" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="H36" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I36" t="s">
+        <v>155</v>
+      </c>
+      <c r="J36" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F37" s="4">
         <v>43668</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="11" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" t="s">
         <v>70</v>
-      </c>
-      <c r="E38" t="s">
-        <v>75</v>
       </c>
       <c r="F38" s="4">
         <v>43668</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F39" s="4">
         <v>43668</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B40" s="6" t="s">
-        <v>118</v>
+    <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E40" t="s">
-        <v>75</v>
-      </c>
-      <c r="F40" s="16">
+        <v>71</v>
+      </c>
+      <c r="F40" s="4">
         <v>43668</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="19" t="s">
-        <v>23</v>
+    <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F41" s="13">
-        <v>43663</v>
+        <v>71</v>
+      </c>
+      <c r="F41" s="4">
+        <v>43668</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H41" s="4">
-        <v>43663</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="K41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F42" s="13">
-        <v>43663</v>
+        <v>71</v>
+      </c>
+      <c r="F42" s="16">
+        <v>43668</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H42" s="4">
-        <v>43663</v>
-      </c>
-      <c r="I42" t="s">
-        <v>103</v>
-      </c>
-      <c r="J42" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F43" s="13">
         <v>43663</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H43" s="4">
         <v>43663</v>
       </c>
-      <c r="I43" t="s">
-        <v>99</v>
-      </c>
-      <c r="J43" t="s">
-        <v>132</v>
+      <c r="I43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="K43" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="19"/>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
         <v>24</v>
       </c>
       <c r="E44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F44" s="13">
         <v>43663</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H44" s="4">
         <v>43663</v>
       </c>
       <c r="I44" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J44" t="s">
-        <v>133</v>
-      </c>
-      <c r="K44" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="19"/>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F45" s="13">
         <v>43663</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="H45" s="4">
         <v>43663</v>
       </c>
       <c r="I45" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J45" t="s">
-        <v>134</v>
+        <v>128</v>
+      </c>
+      <c r="K45" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="19"/>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F46" s="13">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="H46" s="4">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="I46" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J46" t="s">
-        <v>135</v>
+        <v>129</v>
+      </c>
+      <c r="K46" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="19"/>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="13">
+        <v>43663</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H47" s="4">
+        <v>43663</v>
+      </c>
+      <c r="I47" t="s">
+        <v>99</v>
+      </c>
+      <c r="J47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="19"/>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" t="s">
         <v>25</v>
       </c>
-      <c r="E47" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47" s="13">
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="13">
         <v>43664</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H47" s="4">
+      <c r="G48" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" s="4">
         <v>43664</v>
       </c>
-      <c r="I47" t="s">
-        <v>92</v>
-      </c>
-      <c r="J47" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B48" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48" t="s">
-        <v>76</v>
-      </c>
-      <c r="F48" s="4">
-        <v>43669</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H48" s="4"/>
+      <c r="I48" t="s">
+        <v>99</v>
+      </c>
+      <c r="J48" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="6"/>
+      <c r="B49" s="19"/>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="D49" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="E49" t="s">
-        <v>77</v>
-      </c>
-      <c r="F49" s="4">
-        <v>43669</v>
+        <v>35</v>
+      </c>
+      <c r="F49" s="13">
+        <v>43664</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H49" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="H49" s="4">
+        <v>43664</v>
+      </c>
+      <c r="I49" t="s">
+        <v>88</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="50" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E50" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F50" s="4">
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E51" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F51" s="4">
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>60</v>
+        <v>39</v>
+      </c>
+      <c r="C52" t="s">
+        <v>53</v>
       </c>
       <c r="D52" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F52" s="4">
         <v>43670</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
-      <c r="C53" s="2" t="s">
-        <v>61</v>
+      <c r="C53" t="s">
+        <v>54</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F53" s="4">
         <v>43670</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B54" s="7"/>
+      <c r="B54" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="C54" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E54" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F54" s="4">
         <v>43670</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
       <c r="C55" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F55" s="4">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" t="s">
         <v>64</v>
       </c>
-      <c r="D56" t="s">
-        <v>70</v>
-      </c>
       <c r="E56" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F56" s="4">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B57" s="7"/>
       <c r="C57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" t="s">
         <v>65</v>
       </c>
-      <c r="D57" t="s">
-        <v>71</v>
-      </c>
       <c r="E57" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F57" s="4">
         <v>43671</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" t="s">
         <v>66</v>
       </c>
-      <c r="D58" t="s">
-        <v>69</v>
-      </c>
       <c r="E58" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F58" s="4">
         <v>43671</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" t="s">
-        <v>94</v>
+      <c r="B59" s="7"/>
+      <c r="C59" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D59" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="E59" t="s">
-        <v>97</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>107</v>
+        <v>76</v>
+      </c>
+      <c r="F59" s="4">
+        <v>43671</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
-      <c r="C60" t="s">
-        <v>95</v>
+      <c r="C60" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D60" t="s">
+        <v>65</v>
+      </c>
+      <c r="E60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F60" s="4">
+        <v>43671</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="7"/>
+      <c r="C62" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" t="s">
         <v>9</v>
       </c>
-      <c r="E60" t="s">
-        <v>97</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="7"/>
-      <c r="C61" t="s">
-        <v>96</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E62" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="7"/>
+      <c r="C63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" t="s">
         <v>7</v>
       </c>
-      <c r="E61" t="s">
-        <v>97</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H61" s="4"/>
+      <c r="E63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B41:B47"/>
+  <mergeCells count="1">
+    <mergeCell ref="B43:B49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J47" r:id="rId1" display="https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
+    <hyperlink ref="J49" r:id="rId1" display="https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Basket-Controller Test (장바구니관련 부분완료 ~ 장바구니조회 (회원)) _ API Ver 1.95
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4022C912-52FB-47C1-9605-4D623E59B7C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0E382F5E-C99D-4FA2-A5D4-9BC3BC172C71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
@@ -1216,10 +1216,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니추가 API (비회원) (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">프론트엔드 테마작업 및 부분 템플릿화(header,footer) +4H </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1307,10 +1303,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니조회 API (회원)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/basket/member/list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1319,7 +1311,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니조회 API (비회원) (완)</t>
+    <t>장바구니조회 API (비회원) (완) + 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니추가 API (비회원) (완) + 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니조회 API (회원) (완)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1807,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
   <dimension ref="A2:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1867,7 +1867,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="7" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -2099,13 +2099,13 @@
       </c>
       <c r="H13" s="4"/>
       <c r="K13" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -2125,13 +2125,13 @@
     <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F15" s="12">
         <v>43669</v>
@@ -2144,13 +2144,13 @@
     <row r="16" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F16" s="12">
         <v>43669</v>

</xml_diff>

<commit_message>
Basket-Controller Test (장바구니관련 완료) _ API Ver 2.0
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0E382F5E-C99D-4FA2-A5D4-9BC3BC172C71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E85B4248-3E47-4501-8F73-6F369D02C936}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="211">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,10 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/api/basket/remove/{basketNo}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>장바구니
 (Basket-Controller)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,14 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니수정 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니상품삭제 API -</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>주문
 (Order-Controller)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -656,10 +644,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ajax 통신으로 상세 옵션 삭제?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>보류 - 상품수정시 함께</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1212,10 +1196,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니추가 API (회원) (완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">프론트엔드 테마작업 및 부분 템플릿화(header,footer) +4H </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1311,15 +1291,217 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장바구니조회 API (비회원) (완) + 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니추가 API (비회원) (완) + 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장바구니조회 API (회원) (완)</t>
+    <t>/api/basket/remove/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/basket/member/allremove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/basket/nonmember/allremove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%EC%B6%94%EA%B0%80-API-(%ED%9A%8C%EC%9B%90))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%EC%B6%94%EA%B0%80-API-(%EB%B9%84%ED%9A%8C%EC%9B%90)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%EC%A1%B0%ED%9A%8C-API-(%EB%B9%84%ED%9A%8C%EC%9B%90))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%EC%A1%B0%ED%9A%8C-API-(%ED%9A%8C%EC%9B%90))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%EC%83%81%ED%92%88%EC%A0%84%EC%B2%B4%EC%82%AD%EC%A0%9C-API-(%EB%B9%84%ED%9A%8C%EC%9B%90))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%EC%88%98%EB%9F%89%EC%88%98%EC%A0%95-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%ED%8A%B9%EC%A0%95%EC%83%81%ED%92%88-%EC%82%AD%EC%A0%9C-API)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%9E%A5%EB%B0%94%EA%B5%AC%EB%8B%88%EC%83%81%ED%92%88%EC%A0%84%EC%B2%B4%EC%82%AD%EC%A0%9C-API-(%ED%9A%8C%EC%9B%90))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajax 통신으로 상세 옵션 삭제? (삭제 flag?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니추가 API (회원) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니추가 API (비회원) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 추가</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니조회 API (회원) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니조회 API (비회원) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 추가</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니수량수정 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니특정상품삭제 API </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니상품전체삭제 API (회원) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">장바구니상품전체삭제 API (비회원) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(완)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1374,7 +1556,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1390,12 +1572,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1429,7 +1605,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1469,16 +1645,13 @@
     <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1805,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
-  <dimension ref="A2:K63"/>
+  <dimension ref="A2:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1841,33 +2014,33 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -1875,25 +2048,25 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <v>43662</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" s="4">
         <v>43662</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1901,51 +2074,51 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>43662</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="4">
         <v>43662</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="13">
+        <v>43662</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="F5" s="14">
-        <v>43662</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="H5" s="4">
         <v>43662</v>
       </c>
       <c r="I5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1953,25 +2126,25 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>43662</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="4">
         <v>43662</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1979,191 +2152,203 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>43662</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="4">
         <v>43662</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="14">
+        <v>17</v>
+      </c>
+      <c r="F8" s="13">
         <v>43662</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H8" s="4">
         <v>43662</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="5"/>
       <c r="G12" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>15</v>
+      <c r="B13" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F13" s="12">
         <v>43669</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H13" s="4"/>
+      <c r="J13" t="s">
+        <v>194</v>
+      </c>
       <c r="K13" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
+      <c r="B14" s="18"/>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F14" s="12">
         <v>43669</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H14" s="4"/>
+      <c r="J14" t="s">
+        <v>195</v>
+      </c>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+      <c r="B15" s="18"/>
       <c r="C15" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F15" s="12">
         <v>43669</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H15" s="4"/>
+      <c r="J15" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="16" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
+      <c r="B16" s="18"/>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F16" s="12">
         <v>43669</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H16" s="4"/>
+      <c r="J16" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="17" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
+      <c r="B17" s="18"/>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -2171,1136 +2356,1187 @@
       <c r="E17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="12">
         <v>43670</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H17" s="4"/>
+      <c r="J17" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
+      <c r="B18" s="18"/>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="4">
+        <v>191</v>
+      </c>
+      <c r="F18" s="12">
         <v>43670</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="J18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>209</v>
       </c>
       <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F19" s="12">
+        <v>43670</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="J19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18"/>
+      <c r="C20" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>193</v>
+      </c>
+      <c r="F20" s="12">
+        <v>43670</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="J20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="13">
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="12">
         <v>43665</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H19" s="4">
-        <v>43665</v>
-      </c>
-      <c r="I19" t="s">
-        <v>153</v>
-      </c>
-      <c r="J19" t="s">
-        <v>143</v>
-      </c>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" s="13">
-        <v>43665</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="H20" s="4">
-        <v>43665</v>
-      </c>
-      <c r="I20" t="s">
-        <v>155</v>
-      </c>
-      <c r="J20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="13">
-        <v>43665</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H21" s="4">
         <v>43665</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="J21" t="s">
-        <v>147</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>142</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="13">
+        <v>113</v>
+      </c>
+      <c r="F22" s="12">
         <v>43665</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H22" s="4">
         <v>43665</v>
       </c>
       <c r="I22" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J22" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
       <c r="C23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="12">
+        <v>43665</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="E23" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" s="13">
-        <v>43665</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="H23" s="4">
         <v>43665</v>
       </c>
       <c r="I23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="12">
+        <v>43665</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I24" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="13">
+      <c r="J24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+      <c r="C25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="12">
+        <v>43665</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I25" t="s">
+        <v>152</v>
+      </c>
+      <c r="J25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="12">
         <v>43668</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H24" s="4">
-        <v>43668</v>
-      </c>
-      <c r="I24" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24" t="s">
-        <v>162</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17"/>
-      <c r="C25" t="s">
-        <v>167</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" t="s">
-        <v>172</v>
-      </c>
-      <c r="F25" s="13">
-        <v>43668</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="4">
-        <v>43668</v>
-      </c>
-      <c r="I25" t="s">
-        <v>160</v>
-      </c>
-      <c r="J25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
-      <c r="C26" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" t="s">
-        <v>158</v>
-      </c>
-      <c r="F26" s="13">
-        <v>43668</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="H26" s="4">
         <v>43668</v>
       </c>
       <c r="I26" t="s">
-        <v>159</v>
+        <v>75</v>
       </c>
       <c r="J26" t="s">
-        <v>164</v>
+        <v>158</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
+      <c r="B27" s="16"/>
       <c r="C27" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>161</v>
-      </c>
-      <c r="F27" s="13">
+        <v>168</v>
+      </c>
+      <c r="F27" s="12">
         <v>43668</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H27" s="4">
         <v>43668</v>
       </c>
       <c r="I27" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="J27" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="13">
-        <v>43669</v>
+        <v>154</v>
+      </c>
+      <c r="F28" s="12">
+        <v>43668</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H28" s="4">
-        <v>43669</v>
+        <v>43668</v>
       </c>
       <c r="I28" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="J28" t="s">
-        <v>179</v>
-      </c>
-      <c r="K28" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>170</v>
-      </c>
-      <c r="F29" s="13">
+        <v>157</v>
+      </c>
+      <c r="F29" s="12">
+        <v>43668</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="4">
+        <v>43668</v>
+      </c>
+      <c r="I29" t="s">
+        <v>169</v>
+      </c>
+      <c r="J29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="7"/>
+      <c r="C30" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="12">
         <v>43669</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H29" s="4">
+      <c r="G30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="4">
         <v>43669</v>
       </c>
-      <c r="I29" t="s">
-        <v>174</v>
-      </c>
-      <c r="J29" t="s">
-        <v>182</v>
-      </c>
-      <c r="K29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
-      <c r="C30" t="s">
-        <v>185</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="13">
-        <v>43669</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="H30" s="4">
-        <v>43670</v>
-      </c>
       <c r="I30" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="J30" t="s">
-        <v>183</v>
+        <v>175</v>
+      </c>
+      <c r="K30" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="12">
+        <v>43669</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" s="4">
+        <v>43669</v>
+      </c>
+      <c r="I31" t="s">
+        <v>170</v>
+      </c>
+      <c r="J31" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="17"/>
+      <c r="C32" t="s">
+        <v>181</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="12">
+        <v>43669</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H32" s="4">
+        <v>43670</v>
+      </c>
+      <c r="I32" t="s">
+        <v>173</v>
+      </c>
+      <c r="J32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="7"/>
+      <c r="C33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D33" t="s">
         <v>4</v>
       </c>
-      <c r="E31" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" s="13">
+      <c r="E33" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="12">
         <v>43669</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="G33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="4">
         <v>43670</v>
       </c>
-      <c r="I31" t="s">
-        <v>178</v>
-      </c>
-      <c r="J31" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="13">
+      <c r="I33" t="s">
+        <v>174</v>
+      </c>
+      <c r="J33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="12">
         <v>43665</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H32" s="4">
-        <v>43665</v>
-      </c>
-      <c r="I32" t="s">
-        <v>153</v>
-      </c>
-      <c r="J32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="8"/>
-      <c r="C33" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="13">
-        <v>43665</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H33" s="4">
-        <v>43665</v>
-      </c>
-      <c r="I33" t="s">
-        <v>153</v>
-      </c>
-      <c r="J33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="6"/>
-      <c r="C34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34" s="13">
-        <v>43665</v>
-      </c>
       <c r="G34" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H34" s="4">
         <v>43665</v>
       </c>
       <c r="I34" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="J34" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="6"/>
+      <c r="B35" s="8"/>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E35" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="12">
         <v>43665</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H35" s="4">
         <v>43665</v>
       </c>
       <c r="I35" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="J35" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6"/>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" s="13">
+        <v>35</v>
+      </c>
+      <c r="F36" s="12">
         <v>43665</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H36" s="4">
         <v>43665</v>
       </c>
       <c r="I36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J36" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="B37" s="6"/>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E37" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="4">
-        <v>43668</v>
+        <v>35</v>
+      </c>
+      <c r="F37" s="12">
+        <v>43665</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H37" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="H37" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I37" t="s">
+        <v>151</v>
+      </c>
+      <c r="J37" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="11" t="s">
-        <v>111</v>
-      </c>
+      <c r="B38" s="6"/>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="4">
-        <v>43668</v>
+        <v>35</v>
+      </c>
+      <c r="F38" s="12">
+        <v>43665</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H38" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="H38" s="4">
+        <v>43665</v>
+      </c>
+      <c r="I38" t="s">
+        <v>151</v>
+      </c>
+      <c r="J38" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F39" s="4">
         <v>43668</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F40" s="4">
         <v>43668</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F41" s="4">
         <v>43668</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B42" s="6" t="s">
-        <v>114</v>
+    <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="16">
+        <v>68</v>
+      </c>
+      <c r="F42" s="4">
         <v>43668</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="19" t="s">
+    <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="4">
+        <v>43668</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="B44" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="15">
+        <v>43668</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" t="s">
         <v>21</v>
       </c>
-      <c r="C43" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" t="s">
-        <v>33</v>
-      </c>
-      <c r="F43" s="13">
+      <c r="E45" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="12">
         <v>43663</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H43" s="4">
-        <v>43663</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="K43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="19"/>
-      <c r="C44" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" s="13">
-        <v>43663</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H44" s="4">
-        <v>43663</v>
-      </c>
-      <c r="I44" t="s">
-        <v>99</v>
-      </c>
-      <c r="J44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="19"/>
-      <c r="C45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="13">
-        <v>43663</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H45" s="4">
         <v>43663</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K45" t="s">
         <v>95</v>
       </c>
-      <c r="J45" t="s">
-        <v>128</v>
-      </c>
-      <c r="K45" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="19"/>
+      <c r="B46" s="18"/>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>34</v>
-      </c>
-      <c r="F46" s="13">
+        <v>32</v>
+      </c>
+      <c r="F46" s="12">
         <v>43663</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H46" s="4">
         <v>43663</v>
       </c>
       <c r="I46" t="s">
+        <v>96</v>
+      </c>
+      <c r="J46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="18"/>
+      <c r="C47" t="s">
         <v>99</v>
-      </c>
-      <c r="J46" t="s">
-        <v>129</v>
-      </c>
-      <c r="K46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="19"/>
-      <c r="C47" t="s">
-        <v>108</v>
       </c>
       <c r="D47" t="s">
         <v>24</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47" s="13">
+        <v>32</v>
+      </c>
+      <c r="F47" s="12">
         <v>43663</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="H47" s="4">
         <v>43663</v>
       </c>
       <c r="I47" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="J47" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="K47" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="19"/>
+      <c r="B48" s="18"/>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
-      </c>
-      <c r="F48" s="13">
-        <v>43664</v>
+        <v>33</v>
+      </c>
+      <c r="F48" s="12">
+        <v>43663</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="H48" s="4">
-        <v>43664</v>
+        <v>43663</v>
       </c>
       <c r="I48" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J48" t="s">
-        <v>131</v>
+        <v>125</v>
+      </c>
+      <c r="K48" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="19"/>
+      <c r="B49" s="18"/>
       <c r="C49" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
       </c>
       <c r="E49" t="s">
-        <v>35</v>
-      </c>
-      <c r="F49" s="13">
+        <v>33</v>
+      </c>
+      <c r="F49" s="12">
+        <v>43663</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H49" s="4">
+        <v>43663</v>
+      </c>
+      <c r="I49" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="18"/>
+      <c r="C50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="12">
         <v>43664</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H49" s="4">
+      <c r="G50" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H50" s="4">
         <v>43664</v>
       </c>
-      <c r="I49" t="s">
-        <v>88</v>
-      </c>
-      <c r="J49" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B50" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" t="s">
-        <v>67</v>
-      </c>
-      <c r="E50" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" s="4">
-        <v>43669</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H50" s="4"/>
+      <c r="I50" t="s">
+        <v>96</v>
+      </c>
+      <c r="J50" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="6"/>
+      <c r="B51" s="18"/>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="D51" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
-      </c>
-      <c r="F51" s="4">
-        <v>43669</v>
+        <v>34</v>
+      </c>
+      <c r="F51" s="12">
+        <v>43664</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H51" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="H51" s="4">
+        <v>43664</v>
+      </c>
+      <c r="I51" t="s">
+        <v>85</v>
+      </c>
+      <c r="J51" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="52" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D52" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F52" s="4">
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="7"/>
+      <c r="B53" s="6"/>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E53" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F53" s="4">
-        <v>43670</v>
+        <v>43669</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B54" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E54" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F54" s="4">
         <v>43670</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
-      <c r="C55" s="2" t="s">
-        <v>57</v>
+      <c r="C55" t="s">
+        <v>51</v>
       </c>
       <c r="D55" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F55" s="4">
         <v>43670</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="B56" s="7"/>
+      <c r="B56" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="C56" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E56" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F56" s="4">
         <v>43670</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B57" s="7"/>
       <c r="C57" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E57" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F57" s="4">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E58" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F58" s="4">
-        <v>43671</v>
+        <v>43670</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
       <c r="C59" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D59" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E59" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F59" s="4">
         <v>43671</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F60" s="4">
         <v>43671</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" t="s">
-        <v>90</v>
+      <c r="B61" s="7"/>
+      <c r="C61" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="E61" t="s">
-        <v>93</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>103</v>
+        <v>73</v>
+      </c>
+      <c r="F61" s="4">
+        <v>43671</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="7"/>
-      <c r="C62" t="s">
-        <v>91</v>
+      <c r="C62" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D62" t="s">
+        <v>62</v>
+      </c>
+      <c r="E62" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="4">
+        <v>43671</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>90</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="7"/>
+      <c r="C64" t="s">
+        <v>88</v>
+      </c>
+      <c r="D64" t="s">
         <v>9</v>
       </c>
-      <c r="E62" t="s">
-        <v>93</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="7"/>
-      <c r="C63" t="s">
-        <v>92</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E64" t="s">
+        <v>90</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="7"/>
+      <c r="C65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D65" t="s">
         <v>7</v>
       </c>
-      <c r="E63" t="s">
-        <v>93</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H63" s="4"/>
+      <c r="E65" t="s">
+        <v>90</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H65" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B43:B49"/>
+  <mergeCells count="2">
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="B13:B20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J49" r:id="rId1" display="https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
+    <hyperlink ref="J51" r:id="rId1" display="https://github.com/skok1025/ShoppingMall-2week-/wiki/%EA%B4%80%EB%A6%AC%EC%9E%90-%EC%83%81%ED%92%88-%EC%B9%B4%ED%85%8C%EA%B3%A0%EB%A6%AC-%EB%AA%A9%EB%A1%9D-%EC%A1%B0%ED%9A%8C-API" xr:uid="{E8640821-409B-478D-A269-AE2CB9CD06B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Admin-Controller Test (관리자 회원관리 완료) _ API Ver 2.1
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E85B4248-3E47-4501-8F73-6F369D02C936}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C1FC99F4-3C36-4CC5-A70C-2010FAB4E2D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -231,14 +231,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관리자 회원 정보 조회 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 회원 정보 삭제 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>관리자 진열 관리
 (Admin-Controller)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1502,6 +1494,14 @@
       </rPr>
       <t>(완)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 회원 정보 삭제 API (완)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 회원 정보 조회 API (완)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1980,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
   <dimension ref="A2:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2029,7 +2029,7 @@
         <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" x14ac:dyDescent="0.3">
@@ -2040,7 +2040,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -2058,15 +2058,15 @@
         <v>43662</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -2084,41 +2084,41 @@
         <v>43662</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="13">
         <v>43662</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H5" s="4">
         <v>43662</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -2136,15 +2136,15 @@
         <v>43662</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="66" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -2162,15 +2162,15 @@
         <v>43662</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -2182,16 +2182,16 @@
         <v>43662</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H8" s="4">
         <v>43662</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2202,13 +2202,13 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2219,13 +2219,13 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2236,19 +2236,19 @@
         <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="5"/>
       <c r="G12" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2256,99 +2256,99 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F13" s="12">
         <v>43669</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H13" s="4"/>
       <c r="J13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18"/>
       <c r="C14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F14" s="12">
         <v>43669</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H14" s="4"/>
       <c r="J14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
       <c r="C15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F15" s="12">
         <v>43669</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H15" s="4"/>
       <c r="J15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18"/>
       <c r="C16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F16" s="12">
         <v>43669</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H16" s="4"/>
       <c r="J16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="18"/>
       <c r="C17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -2360,77 +2360,77 @@
         <v>43670</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H17" s="4"/>
       <c r="J17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="18"/>
       <c r="C18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F18" s="12">
         <v>43670</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H18" s="4"/>
       <c r="J18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="18"/>
       <c r="C19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F19" s="12">
         <v>43670</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H19" s="4"/>
       <c r="J19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="18"/>
       <c r="C20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F20" s="12">
         <v>43670</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H20" s="4"/>
       <c r="J20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -2438,7 +2438,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -2450,116 +2450,116 @@
         <v>43665</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H21" s="4">
         <v>43665</v>
       </c>
       <c r="I21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F22" s="12">
         <v>43665</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H22" s="4">
         <v>43665</v>
       </c>
       <c r="I22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F23" s="12">
         <v>43665</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H23" s="4">
         <v>43665</v>
       </c>
       <c r="I23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10"/>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F24" s="12">
         <v>43665</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H24" s="4">
         <v>43665</v>
       </c>
       <c r="I24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F25" s="12">
         <v>43665</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H25" s="4">
         <v>43665</v>
       </c>
       <c r="I25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -2567,226 +2567,226 @@
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F26" s="12">
         <v>43668</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H26" s="4">
         <v>43668</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="16"/>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F27" s="12">
         <v>43668</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H27" s="4">
         <v>43668</v>
       </c>
       <c r="I27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J27" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F28" s="12">
         <v>43668</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H28" s="4">
         <v>43668</v>
       </c>
       <c r="I28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F29" s="12">
         <v>43668</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H29" s="4">
         <v>43668</v>
       </c>
       <c r="I29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30" s="12">
         <v>43669</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H30" s="4">
         <v>43669</v>
       </c>
       <c r="I30" t="s">
+        <v>167</v>
+      </c>
+      <c r="J30" t="s">
+        <v>173</v>
+      </c>
+      <c r="K30" t="s">
         <v>169</v>
-      </c>
-      <c r="J30" t="s">
-        <v>175</v>
-      </c>
-      <c r="K30" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F31" s="12">
         <v>43669</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H31" s="4">
         <v>43669</v>
       </c>
       <c r="I31" t="s">
+        <v>168</v>
+      </c>
+      <c r="J31" t="s">
+        <v>176</v>
+      </c>
+      <c r="K31" t="s">
         <v>170</v>
-      </c>
-      <c r="J31" t="s">
-        <v>178</v>
-      </c>
-      <c r="K31" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="17"/>
       <c r="C32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F32" s="12">
         <v>43669</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H32" s="4">
         <v>43670</v>
       </c>
       <c r="I32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F33" s="12">
         <v>43669</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H33" s="4">
         <v>43670</v>
       </c>
       <c r="I33" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -2797,7 +2797,7 @@
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D34" t="s">
         <v>21</v>
@@ -2809,22 +2809,22 @@
         <v>43665</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H34" s="4">
         <v>43665</v>
       </c>
       <c r="I34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="8"/>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -2836,22 +2836,22 @@
         <v>43665</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H35" s="4">
         <v>43665</v>
       </c>
       <c r="I35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6"/>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
@@ -2863,22 +2863,22 @@
         <v>43665</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H36" s="4">
         <v>43665</v>
       </c>
       <c r="I36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
@@ -2890,22 +2890,22 @@
         <v>43665</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H37" s="4">
         <v>43665</v>
       </c>
       <c r="I37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6"/>
       <c r="C38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D38" t="s">
         <v>24</v>
@@ -2917,21 +2917,21 @@
         <v>43665</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H38" s="4">
         <v>43665</v>
       </c>
       <c r="I38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
         <v>40</v>
@@ -2940,118 +2940,118 @@
         <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F39" s="4">
         <v>43668</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
         <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F40" s="4">
         <v>43668</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
         <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F41" s="4">
         <v>43668</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
         <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F42" s="4">
         <v>43668</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s">
         <v>44</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F43" s="4">
         <v>43668</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H43" s="4"/>
     </row>
     <row r="44" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B44" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F44" s="15">
         <v>43668</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H44" s="4"/>
     </row>
@@ -3060,7 +3060,7 @@
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D45" t="s">
         <v>21</v>
@@ -3072,25 +3072,25 @@
         <v>43663</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H45" s="4">
         <v>43663</v>
       </c>
       <c r="I45" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="K45" t="s">
         <v>93</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K45" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="18"/>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
         <v>23</v>
@@ -3102,22 +3102,22 @@
         <v>43663</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H46" s="4">
         <v>43663</v>
       </c>
       <c r="I46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J46" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="18"/>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
         <v>24</v>
@@ -3129,25 +3129,25 @@
         <v>43663</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H47" s="4">
         <v>43663</v>
       </c>
       <c r="I47" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="18"/>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
         <v>21</v>
@@ -3159,25 +3159,25 @@
         <v>43663</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H48" s="4">
         <v>43663</v>
       </c>
       <c r="I48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K48" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="18"/>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
@@ -3189,22 +3189,22 @@
         <v>43663</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H49" s="4">
         <v>43663</v>
       </c>
       <c r="I49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="18"/>
       <c r="C50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
         <v>24</v>
@@ -3216,22 +3216,22 @@
         <v>43664</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H50" s="4">
         <v>43664</v>
       </c>
       <c r="I50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J50" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="18"/>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -3243,16 +3243,16 @@
         <v>43664</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H51" s="4">
         <v>43664</v>
       </c>
       <c r="I51" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J51" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
@@ -3263,16 +3263,16 @@
         <v>37</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F52" s="4">
         <v>43669</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H52" s="4"/>
     </row>
@@ -3282,16 +3282,16 @@
         <v>46</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F53" s="4">
         <v>43669</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H53" s="4"/>
     </row>
@@ -3300,229 +3300,229 @@
         <v>38</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>210</v>
       </c>
       <c r="D54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F54" s="4">
         <v>43670</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7"/>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F55" s="4">
         <v>43670</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B56" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E56" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F56" s="4">
         <v>43670</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B57" s="7"/>
       <c r="C57" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E57" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F57" s="4">
         <v>43670</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E58" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F58" s="4">
         <v>43670</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:11" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
       <c r="C59" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F59" s="4">
         <v>43671</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F60" s="4">
         <v>43671</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="7"/>
       <c r="C61" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F61" s="4">
         <v>43671</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="7"/>
       <c r="C62" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F62" s="4">
         <v>43671</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D63" t="s">
         <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="7"/>
       <c r="C64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H64" s="4"/>
     </row>
     <row r="65" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
       <c r="C65" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
ERD VERSION 별 폴더 추가
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6C92EF66-1811-4FDC-AD5C-458278BA6BAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{492C33AC-A820-4FA7-BC79-D922912B4764}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="29100" windowHeight="16500" xr2:uid="{5B0FA2CB-56EF-4680-897A-8EB9FC9E2468}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="241">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1809,11 +1809,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전체 상품리스트 조회 API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/goods/list/{startNo}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 상품리스트 조회 API + 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[링크](https://github.com/skok1025/ShoppingMall/wiki/%EC%A0%84%EC%B2%B4-%EC%83%81%ED%92%88%EB%A6%AC%EC%8A%A4%ED%8A%B8-%EC%A1%B0%ED%9A%8C-API)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2304,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E3AA6-FD47-4EA7-8BF3-D661425B9730}">
   <dimension ref="A2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2317,7 +2325,7 @@
     <col min="6" max="6" width="10.625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="255.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="48.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2816,17 +2824,29 @@
     <row r="21" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="20"/>
       <c r="C21" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D21" t="s">
         <v>236</v>
       </c>
       <c r="E21" t="s">
+        <v>237</v>
+      </c>
+      <c r="F21" s="11">
+        <v>43679</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4">
+        <v>43679</v>
+      </c>
+      <c r="I21" t="s">
+        <v>238</v>
+      </c>
+      <c r="J21" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="22" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8"/>

</xml_diff>